<commit_message>
Fix README.md formatting and remove unused code
</commit_message>
<xml_diff>
--- a/data/output/performance_Close_BTC.xlsx
+++ b/data/output/performance_Close_BTC.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,61 +448,101 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Root Mean Square Error</t>
+          <t>Mean Square Error</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.04732704134909583</v>
+        <v>2243454.062</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mean Absolute Error</t>
+          <t>Root Mean Square Error</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0328422671053074</v>
+        <v>1497.816</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mean Absolute Percentage Error</t>
+          <t>Mean Absolute Error</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.271983367858482</v>
+        <v>1272.794</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>U-Theil1 Statistic</t>
+          <t>Root Mean Square Error (log)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>67.66785424618668</v>
+        <v>0.047</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>U-Theil2 Statistic</t>
+          <t>Mean Absolute Error (log)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2103585054355269</v>
+        <v>0.033</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Mean Absolute Percentage Error</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6.272</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>U-Theil1 Statistic</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>67.66800000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>U-Theil2 Statistic</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Diebold-Mariano Test</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>35.59074660663671</v>
+      <c r="B10" t="n">
+        <v>35.591</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Rendement Absolue</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>